<commit_message>
adding tsne and xgboost
</commit_message>
<xml_diff>
--- a/0 - Revisão Python/Pandas/Excel_Sample.xlsx
+++ b/0 - Revisão Python/Pandas/Excel_Sample.xlsx
@@ -14,14 +14,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -34,9 +43,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -49,9 +55,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
   </si>
   <si>
     <t>d</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>7</t>
@@ -438,16 +438,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -456,16 +456,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -473,16 +473,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -490,13 +490,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -507,13 +507,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -524,13 +524,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>

</xml_diff>